<commit_message>
Update 132 lab list for 2020fall.xlsx
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020fall.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020fall.xlsx
@@ -986,7 +986,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="240">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1657,13 +1657,6 @@
     <t>2020 spr Jerry</t>
   </si>
   <si>
-    <t>2020 spr Jack</t>
-  </si>
-  <si>
-    <t>2020 
-Matt</t>
-  </si>
-  <si>
     <t>2019 fall Christine</t>
   </si>
   <si>
@@ -1701,6 +1694,21 @@
   </si>
   <si>
     <t>Needed for kinetic theory labs?</t>
+  </si>
+  <si>
+    <t>2020 fall Jack</t>
+  </si>
+  <si>
+    <t>2020 fall Matt</t>
+  </si>
+  <si>
+    <t>lightly edited by MT, 2020</t>
+  </si>
+  <si>
+    <t>The Resistor Color Code</t>
+  </si>
+  <si>
+    <t>by MT 2020</t>
   </si>
 </sst>
 </file>
@@ -2904,11 +2912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD119"/>
+  <dimension ref="A1:AD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2976,16 +2984,16 @@
         <v>212</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q1" s="47" t="s">
         <v>221</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="T1" s="47" t="s">
         <v>219</v>
@@ -3586,7 +3594,7 @@
     </row>
     <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>205</v>
@@ -3602,7 +3610,7 @@
         <v>4</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L12" s="75"/>
       <c r="M12" s="75"/>
@@ -3613,14 +3621,11 @@
         <v>1</v>
       </c>
       <c r="S12" s="77">
-        <v>1</v>
-      </c>
-      <c r="T12" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U12" s="67">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V12" s="31"/>
       <c r="W12" s="42">
@@ -3636,7 +3641,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>205</v>
@@ -3652,7 +3657,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L13" s="75"/>
       <c r="M13" s="75"/>
@@ -3663,14 +3668,11 @@
         <v>1</v>
       </c>
       <c r="S13" s="77">
-        <v>1</v>
-      </c>
-      <c r="T13" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U13" s="67">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V13" s="31"/>
       <c r="W13" s="31"/>
@@ -3684,7 +3686,7 @@
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>205</v>
@@ -3700,7 +3702,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L14" s="75"/>
       <c r="M14" s="75"/>
@@ -3722,7 +3724,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>205</v>
@@ -3738,7 +3740,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L15" s="75"/>
       <c r="M15" s="75"/>
@@ -4391,16 +4393,16 @@
         <v>0</v>
       </c>
       <c r="X26" s="6">
-        <f t="shared" ref="X26:X34" si="2">SUMIF(U$2:U$82,"&gt;=" &amp; W26,F$2:F$82)</f>
-        <v>356</v>
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W26,F$2:F$83)</f>
+        <v>358</v>
       </c>
       <c r="Y26" s="6">
-        <f t="shared" ref="Y26:Y34" si="3">SUMIF(U$2:U$82,"&gt;=" &amp; W26,E$2:E$82)</f>
-        <v>28</v>
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W26,E$2:E$83)</f>
+        <v>29</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" ref="Z26:Z34" si="4">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
-        <v>37.960000000000008</v>
+        <f t="shared" ref="Z26:Z34" si="2">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
+        <v>38.480000000000004</v>
       </c>
       <c r="AA26" s="31"/>
       <c r="AB26" s="31"/>
@@ -4463,16 +4465,16 @@
         <v>0.5</v>
       </c>
       <c r="X27" s="6">
-        <f t="shared" si="2"/>
-        <v>278</v>
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W27,F$2:F$83)</f>
+        <v>280</v>
       </c>
       <c r="Y27" s="6">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W27,E$2:E$83)</f>
+        <v>26</v>
       </c>
       <c r="Z27" s="8">
         <f>($Y$17 + $Y$15*X27+$Y$16*Y27)*(1+Y$18+Y$19)</f>
-        <v>31.72</v>
+        <v>32.24</v>
       </c>
       <c r="AA27" s="31"/>
       <c r="AB27" s="31"/>
@@ -4541,16 +4543,16 @@
         <v>1</v>
       </c>
       <c r="X28" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W28,F$2:F$83)</f>
+        <v>264</v>
+      </c>
+      <c r="Y28" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W28,E$2:E$83)</f>
+        <v>23</v>
+      </c>
+      <c r="Z28" s="8">
         <f t="shared" si="2"/>
-        <v>262</v>
-      </c>
-      <c r="Y28" s="6">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="Z28" s="8">
-        <f t="shared" si="4"/>
-        <v>29.510000000000005</v>
+        <v>30.03</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -4593,16 +4595,16 @@
         <v>1.5</v>
       </c>
       <c r="X29" s="29">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W29,F$2:F$83)</f>
+        <v>162</v>
+      </c>
+      <c r="Y29" s="29">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W29,E$2:E$83)</f>
+        <v>17</v>
+      </c>
+      <c r="Z29" s="8">
         <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="Y29" s="29">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="Z29" s="8">
-        <f t="shared" si="4"/>
-        <v>20.540000000000003</v>
+        <v>21.06</v>
       </c>
       <c r="AA29" s="31"/>
       <c r="AB29" s="31"/>
@@ -4647,16 +4649,16 @@
         <v>2</v>
       </c>
       <c r="X30" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W30,F$2:F$83)</f>
+        <v>158</v>
+      </c>
+      <c r="Y30" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W30,E$2:E$83)</f>
+        <v>17</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="2"/>
-        <v>156</v>
-      </c>
-      <c r="Y30" s="6">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="Z30" s="8">
-        <f t="shared" si="4"/>
-        <v>20.28</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -4708,16 +4710,16 @@
         <v>2.5</v>
       </c>
       <c r="X31" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W31,F$2:F$83)</f>
+        <v>68</v>
+      </c>
+      <c r="Y31" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W31,E$2:E$83)</f>
+        <v>6</v>
+      </c>
+      <c r="Z31" s="8">
         <f t="shared" si="2"/>
-        <v>76</v>
-      </c>
-      <c r="Y31" s="6">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="Z31" s="8">
-        <f t="shared" si="4"/>
-        <v>11.57</v>
+        <v>10.66</v>
       </c>
       <c r="AA31" s="31"/>
       <c r="AB31" s="31"/>
@@ -4789,16 +4791,16 @@
         <v>3</v>
       </c>
       <c r="X32" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W32,F$2:F$83)</f>
+        <v>64</v>
+      </c>
+      <c r="Y32" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W32,E$2:E$83)</f>
+        <v>6</v>
+      </c>
+      <c r="Z32" s="8">
         <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="Y32" s="6">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="Z32" s="8">
-        <f t="shared" si="4"/>
-        <v>11.309999999999999</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="33" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4862,16 +4864,16 @@
         <v>3.5</v>
       </c>
       <c r="X33" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W33,F$2:F$83)</f>
+        <v>8</v>
+      </c>
+      <c r="Y33" s="6">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W33,E$2:E$83)</f>
+        <v>2</v>
+      </c>
+      <c r="Z33" s="8">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="Y33" s="6">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="Z33" s="8">
-        <f t="shared" si="4"/>
-        <v>6.1099999999999994</v>
+        <v>5.2</v>
       </c>
       <c r="AA33"/>
       <c r="AB33"/>
@@ -4892,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="13">
-        <f t="shared" ref="F34:F65" si="5">CEILING(D34,W$22+1)</f>
+        <f t="shared" ref="F34:F65" si="3">CEILING(D34,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G34" s="13">
@@ -4943,16 +4945,16 @@
         <v>4</v>
       </c>
       <c r="X34" s="45">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W34,F$2:F$83)</f>
+        <v>8</v>
+      </c>
+      <c r="Y34" s="45">
+        <f>SUMIF(U$2:U$83,"&gt;=" &amp; W34,E$2:E$83)</f>
+        <v>2</v>
+      </c>
+      <c r="Z34" s="9">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="Y34" s="45">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="Z34" s="9">
-        <f t="shared" si="4"/>
-        <v>6.1099999999999994</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="35" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -4970,7 +4972,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G35" s="13">
@@ -5026,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H36" s="13">
@@ -5080,7 +5082,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J37" s="13">
@@ -5127,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J38" s="13">
@@ -5178,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G39" s="13">
@@ -5193,7 +5195,9 @@
       <c r="J39" s="13">
         <v>21</v>
       </c>
-      <c r="K39" s="21"/>
+      <c r="K39" s="21" t="s">
+        <v>237</v>
+      </c>
       <c r="L39" s="32">
         <v>1</v>
       </c>
@@ -5243,7 +5247,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G40" s="12" t="s">
@@ -5307,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G41" s="13">
@@ -5367,7 +5371,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G42" s="13"/>
@@ -5414,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H43" s="13">
@@ -5467,7 +5471,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G44" s="13" t="s">
@@ -5528,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G45" s="12" t="s">
@@ -5544,7 +5548,7 @@
         <v>26</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L45" s="33">
         <v>1</v>
@@ -5588,7 +5592,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G46" s="13"/>
@@ -5631,7 +5635,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G47" s="13" t="s">
@@ -5647,7 +5651,7 @@
         <v>27</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L47" s="32">
         <v>1</v>
@@ -5693,7 +5697,7 @@
         <v>4</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G48" s="13"/>
@@ -5742,7 +5746,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G49" s="13">
@@ -5808,7 +5812,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G50" s="13">
@@ -5862,7 +5866,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G51" s="12">
@@ -5914,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G52" s="13">
@@ -5976,7 +5980,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G53" s="12"/>
@@ -6030,7 +6034,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G54" s="13">
@@ -6095,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G55" s="13">
@@ -6143,7 +6147,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G56" s="13">
@@ -6184,7 +6188,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G57" s="13">
@@ -6242,7 +6246,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G58" s="13">
@@ -6300,7 +6304,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G59" s="13">
@@ -6356,7 +6360,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H60" s="13">
@@ -6413,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J61" s="13">
@@ -6454,7 +6458,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J62" s="13">
@@ -6499,7 +6503,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G63" s="13">
@@ -6535,7 +6539,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G64" s="13">
@@ -6575,7 +6579,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J65" s="13">
@@ -6623,7 +6627,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="12">
-        <f t="shared" ref="F66:F81" si="6">CEILING(D66,W$22+1)</f>
+        <f t="shared" ref="F66:F82" si="4">CEILING(D66,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G66" s="12">
@@ -6680,7 +6684,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G67" s="13">
@@ -6702,7 +6706,7 @@
       <c r="S67" s="77"/>
       <c r="T67" s="75"/>
       <c r="U67" s="67">
-        <f t="shared" ref="U67:U81" si="7">SUM(Q67:T67)</f>
+        <f t="shared" ref="U67:U82" si="5">SUM(Q67:T67)</f>
         <v>1</v>
       </c>
       <c r="V67" s="31"/>
@@ -6729,7 +6733,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G68" s="13">
@@ -6740,7 +6744,7 @@
       <c r="M68" s="31"/>
       <c r="S68" s="77"/>
       <c r="U68" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V68" s="31"/>
@@ -6760,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G69" s="26">
@@ -6784,7 +6788,7 @@
       <c r="S69" s="78"/>
       <c r="T69" s="78"/>
       <c r="U69" s="81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="V69" s="31"/>
@@ -6806,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G70" s="13">
@@ -6817,7 +6821,7 @@
       <c r="M70" s="31"/>
       <c r="S70" s="77"/>
       <c r="U70" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V70" s="31"/>
@@ -6839,7 +6843,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G71" s="13">
@@ -6859,7 +6863,7 @@
       <c r="S71" s="77"/>
       <c r="T71" s="75"/>
       <c r="U71" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V71" s="31"/>
@@ -6886,7 +6890,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K72" s="21" t="s">
@@ -6897,7 +6901,7 @@
       <c r="S72" s="77"/>
       <c r="T72" s="78"/>
       <c r="U72" s="81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V72" s="31"/>
@@ -6921,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G73" s="12"/>
@@ -6951,7 +6955,7 @@
       </c>
       <c r="T73" s="77"/>
       <c r="U73" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W73" s="3"/>
@@ -6976,7 +6980,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K74" s="21" t="s">
@@ -7006,7 +7010,7 @@
       </c>
       <c r="T74" s="77"/>
       <c r="U74" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="V74" s="31"/>
@@ -7024,7 +7028,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G75" s="13"/>
@@ -7052,7 +7056,7 @@
         <v>2</v>
       </c>
       <c r="U75" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W75" s="3"/>
@@ -7068,7 +7072,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K76" s="21"/>
@@ -7094,7 +7098,7 @@
         <v>1</v>
       </c>
       <c r="U76" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="V76" s="31"/>
@@ -7115,7 +7119,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G77" s="13"/>
@@ -7149,7 +7153,7 @@
       </c>
       <c r="T77" s="75"/>
       <c r="U77" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="V77" s="14"/>
@@ -7162,166 +7166,186 @@
       <c r="AC77" s="31"/>
       <c r="AD77" s="31"/>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
       <c r="B78" s="22" t="s">
-        <v>153</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="C78" s="22"/>
       <c r="D78" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E78" s="13">
         <v>1</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="K78" s="21"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="21" t="s">
+        <v>239</v>
+      </c>
       <c r="L78" s="75"/>
-      <c r="M78" s="75"/>
-      <c r="S78" s="77"/>
+      <c r="M78" s="73"/>
+      <c r="N78" s="75"/>
+      <c r="O78" s="75"/>
+      <c r="P78" s="75"/>
+      <c r="Q78" s="75">
+        <v>1</v>
+      </c>
+      <c r="R78" s="75"/>
+      <c r="S78" s="77">
+        <v>1</v>
+      </c>
+      <c r="T78" s="75"/>
       <c r="U78" s="67">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="V78" s="14"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="31"/>
+      <c r="Y78" s="31"/>
+      <c r="Z78" s="31"/>
+      <c r="AA78" s="31"/>
+      <c r="AB78" s="31"/>
+      <c r="AC78" s="31"/>
+      <c r="AD78" s="31"/>
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B79" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D79" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E79" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="K79" s="21"/>
       <c r="L79" s="75"/>
       <c r="M79" s="75"/>
       <c r="S79" s="77"/>
       <c r="U79" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V79" s="14"/>
-      <c r="AA79" s="6"/>
-      <c r="AB79" s="6"/>
-      <c r="AC79" s="6"/>
-      <c r="AD79" s="6"/>
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B80" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D80" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E80" s="13">
         <v>0</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="K80" s="21"/>
       <c r="L80" s="75"/>
       <c r="M80" s="75"/>
       <c r="S80" s="77"/>
       <c r="U80" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V80" s="14"/>
-    </row>
-    <row r="81" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="10"/>
-      <c r="B81" s="23" t="s">
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+      <c r="AC80" s="6"/>
+      <c r="AD80" s="6"/>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B81" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" s="13">
+        <v>4</v>
+      </c>
+      <c r="E81" s="13">
+        <v>0</v>
+      </c>
+      <c r="F81" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K81" s="21"/>
+      <c r="L81" s="75"/>
+      <c r="M81" s="75"/>
+      <c r="S81" s="77"/>
+      <c r="U81" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V81" s="14"/>
+    </row>
+    <row r="82" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="10"/>
+      <c r="B82" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="26">
-        <v>1</v>
-      </c>
-      <c r="E81" s="26">
-        <v>0</v>
-      </c>
-      <c r="F81" s="26">
-        <f t="shared" si="6"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="26">
+        <v>1</v>
+      </c>
+      <c r="E82" s="26">
+        <v>0</v>
+      </c>
+      <c r="F82" s="26">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G81" s="26"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="26"/>
-      <c r="J81" s="26"/>
-      <c r="K81" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="L81" s="35"/>
-      <c r="M81" s="35">
-        <v>1</v>
-      </c>
-      <c r="N81" s="78"/>
-      <c r="O81" s="78">
-        <v>1</v>
-      </c>
-      <c r="P81" s="78">
-        <v>1</v>
-      </c>
-      <c r="Q81" s="78"/>
-      <c r="R81" s="78"/>
-      <c r="S81" s="78"/>
-      <c r="T81" s="78"/>
-      <c r="U81" s="81">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V81" s="14"/>
-      <c r="W81" s="3"/>
-      <c r="X81"/>
-      <c r="Y81"/>
-      <c r="Z81"/>
-      <c r="AA81" s="6"/>
-      <c r="AB81" s="6"/>
-      <c r="AC81" s="6"/>
-      <c r="AD81" s="6"/>
-    </row>
-    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="11"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="K83" s="82"/>
-      <c r="L83" s="63"/>
-      <c r="M83" s="63"/>
-      <c r="N83" s="63"/>
-      <c r="O83" s="63"/>
-      <c r="P83" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q83" s="61">
-        <f t="array" ref="Q83">SUM($F2:$F81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>166</v>
-      </c>
-      <c r="R83" s="61">
-        <f t="array" ref="R83">SUM($F2:$F81*(R2:R81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>152</v>
-      </c>
-      <c r="S83" s="61">
-        <f t="array" ref="S83">SUM($F2:$F81*(S2:S81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>172</v>
-      </c>
-      <c r="T83" s="63"/>
-      <c r="X83" s="31"/>
-      <c r="Y83" s="31"/>
-      <c r="Z83" s="31"/>
-      <c r="AA83" s="6"/>
-      <c r="AB83" s="6"/>
-      <c r="AC83" s="6"/>
-      <c r="AD83" s="6"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="L82" s="35"/>
+      <c r="M82" s="35">
+        <v>1</v>
+      </c>
+      <c r="N82" s="78"/>
+      <c r="O82" s="78">
+        <v>1</v>
+      </c>
+      <c r="P82" s="78">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="78"/>
+      <c r="R82" s="78"/>
+      <c r="S82" s="78"/>
+      <c r="T82" s="78"/>
+      <c r="U82" s="81">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V82" s="14"/>
+      <c r="W82" s="3"/>
+      <c r="X82"/>
+      <c r="Y82"/>
+      <c r="Z82"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
+    </row>
+    <row r="83" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="11"/>
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K84" s="82"/>
@@ -7329,22 +7353,25 @@
       <c r="M84" s="63"/>
       <c r="N84" s="63"/>
       <c r="O84" s="63"/>
-      <c r="P84" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q84" s="63">
-        <f t="array" ref="Q84">SUM($F2:$F81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
+      <c r="P84" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q84" s="61">
+        <f t="array" ref="Q84">SUM($F2:$F82*(Q2:Q82&gt;=0.9)*($U2:$U82&gt;=$W$12))</f>
         <v>168</v>
       </c>
-      <c r="R84" s="63">
-        <f t="array" ref="R84">SUM($F2:$F81*R2:R81*($U2:$U81&gt;=$W$12))</f>
-        <v>152.4</v>
-      </c>
-      <c r="S84" s="63">
-        <f t="array" ref="S84">SUM($F2:$F81*S2:S81*($U2:$U81&gt;=$W$12))</f>
-        <v>175.39999999999998</v>
+      <c r="R84" s="61">
+        <f t="array" ref="R84">SUM($F2:$F82*(R2:R82&gt;=0.9)*($U2:$U82&gt;=$W$12))</f>
+        <v>152</v>
+      </c>
+      <c r="S84" s="61">
+        <f t="array" ref="S84">SUM($F2:$F82*(S2:S82&gt;=0.9)*($U2:$U82&gt;=$W$12))</f>
+        <v>166</v>
       </c>
       <c r="T84" s="63"/>
+      <c r="X84" s="31"/>
+      <c r="Y84" s="31"/>
+      <c r="Z84" s="31"/>
       <c r="AA84" s="6"/>
       <c r="AB84" s="6"/>
       <c r="AC84" s="6"/>
@@ -7357,21 +7384,25 @@
       <c r="N85" s="63"/>
       <c r="O85" s="63"/>
       <c r="P85" s="62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q85" s="63">
-        <f t="array" ref="Q85">SUM($F$2:$F$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
+        <f t="array" ref="Q85">SUM($F2:$F82*Q2:Q82*($U2:$U82&gt;=$W$12))</f>
         <v>170</v>
       </c>
       <c r="R85" s="63">
-        <f t="array" ref="R85">SUM($F$2:$F$81*(R$2:R$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>156</v>
+        <f t="array" ref="R85">SUM($F2:$F82*R2:R82*($U2:$U82&gt;=$W$12))</f>
+        <v>152.4</v>
       </c>
       <c r="S85" s="63">
-        <f t="array" ref="S85">SUM($F$2:$F$81*(S$2:S$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>190</v>
+        <f t="array" ref="S85">SUM($F2:$F82*S2:S82*($U2:$U82&gt;=$W$12))</f>
+        <v>169.39999999999998</v>
       </c>
       <c r="T85" s="63"/>
+      <c r="AA85" s="6"/>
+      <c r="AB85" s="6"/>
+      <c r="AC85" s="6"/>
+      <c r="AD85" s="6"/>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K86" s="82"/>
@@ -7380,161 +7411,184 @@
       <c r="N86" s="63"/>
       <c r="O86" s="63"/>
       <c r="P86" s="62" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q86" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <f t="array" ref="Q86">SUM($F$2:$F$82*(Q$2:Q$82&gt;=0.1)*($U$2:$U$82&gt;=$W$12))</f>
+        <v>172</v>
       </c>
       <c r="R86" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <f t="array" ref="R86">SUM($F$2:$F$82*(R$2:R$82&gt;=0.1)*($U$2:$U$82&gt;=$W$12))</f>
+        <v>156</v>
       </c>
       <c r="S86" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <f t="array" ref="S86">SUM($F$2:$F$82*(S$2:S$82&gt;=0.1)*($U$2:$U$82&gt;=$W$12))</f>
+        <v>184</v>
       </c>
       <c r="T86" s="63"/>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K87" s="82"/>
-      <c r="L87" s="64"/>
-      <c r="M87" s="64"/>
-      <c r="N87" s="64"/>
-      <c r="O87" s="64"/>
+      <c r="L87" s="63"/>
+      <c r="M87" s="63"/>
+      <c r="N87" s="63"/>
+      <c r="O87" s="63"/>
       <c r="P87" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q87" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>264</v>
+      </c>
+      <c r="R87" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>264</v>
+      </c>
+      <c r="S87" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>264</v>
+      </c>
+      <c r="T87" s="63"/>
+    </row>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="K88" s="82"/>
+      <c r="L88" s="64"/>
+      <c r="M88" s="64"/>
+      <c r="N88" s="64"/>
+      <c r="O88" s="64"/>
+      <c r="P88" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="Q87" s="64">
-        <f t="shared" ref="Q87:S87" si="8">Q84/Q86</f>
-        <v>0.64122137404580148</v>
-      </c>
-      <c r="R87" s="64">
-        <f t="shared" si="8"/>
-        <v>0.58167938931297714</v>
-      </c>
-      <c r="S87" s="64">
-        <f t="shared" si="8"/>
-        <v>0.66946564885496174</v>
-      </c>
-      <c r="T87" s="64"/>
-    </row>
-    <row r="88" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D88" s="31"/>
-      <c r="K88" s="82"/>
-      <c r="L88" s="63"/>
-      <c r="M88" s="63"/>
-      <c r="N88" s="63"/>
-      <c r="O88" s="63"/>
-      <c r="P88" s="65" t="s">
+      <c r="Q88" s="64">
+        <f t="shared" ref="Q88:S88" si="6">Q85/Q87</f>
+        <v>0.64393939393939392</v>
+      </c>
+      <c r="R88" s="64">
+        <f t="shared" si="6"/>
+        <v>0.57727272727272727</v>
+      </c>
+      <c r="S88" s="64">
+        <f t="shared" si="6"/>
+        <v>0.64166666666666661</v>
+      </c>
+      <c r="T88" s="64"/>
+    </row>
+    <row r="89" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D89" s="31"/>
+      <c r="K89" s="82"/>
+      <c r="L89" s="63"/>
+      <c r="M89" s="63"/>
+      <c r="N89" s="63"/>
+      <c r="O89" s="63"/>
+      <c r="P89" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="Q88" s="66">
-        <f t="array" ref="Q88">SUM($F2:$F81*Q2:Q81*($U2:$U81&lt;$W$12))</f>
+      <c r="Q89" s="66">
+        <f t="array" ref="Q89">SUM($F2:$F82*Q2:Q82*($U2:$U82&lt;$W$12))</f>
         <v>3</v>
       </c>
-      <c r="R88" s="66">
-        <f t="array" ref="R88">SUM($F2:$F81*R2:R81*($U2:$U81&lt;$W$12))</f>
-        <v>0</v>
-      </c>
-      <c r="S88" s="66">
-        <f t="array" ref="S88">SUM($F2:$F81*S2:S81*($U2:$U81&lt;$W$12))</f>
+      <c r="R89" s="66">
+        <f t="array" ref="R89">SUM($F2:$F82*R2:R82*($U2:$U82&lt;$W$12))</f>
+        <v>0</v>
+      </c>
+      <c r="S89" s="66">
+        <f t="array" ref="S89">SUM($F2:$F82*S2:S82*($U2:$U82&lt;$W$12))</f>
         <v>7.8000000000000007</v>
       </c>
-      <c r="T88" s="63"/>
-      <c r="Z88" s="31"/>
-    </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="D89" s="31"/>
+      <c r="T89" s="63"/>
+      <c r="Z89" s="31"/>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D90" s="31"/>
     </row>
-    <row r="91" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10"/>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="19"/>
-      <c r="L91" s="2"/>
-      <c r="M91" s="2"/>
-      <c r="N91" s="75"/>
-      <c r="O91" s="75"/>
-      <c r="P91" s="75"/>
-      <c r="Q91" s="75"/>
-      <c r="R91" s="75"/>
-      <c r="S91" s="75"/>
-      <c r="T91" s="75"/>
-      <c r="U91" s="3"/>
-      <c r="V91" s="3"/>
-      <c r="W91" s="3"/>
-      <c r="X91"/>
-      <c r="Y91"/>
-      <c r="Z91"/>
-      <c r="AA91"/>
-      <c r="AB91"/>
-      <c r="AC91"/>
-      <c r="AD91"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="N92" s="75" t="s">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="D91" s="31"/>
+    </row>
+    <row r="92" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="19"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="75"/>
+      <c r="O92" s="75"/>
+      <c r="P92" s="75"/>
+      <c r="Q92" s="75"/>
+      <c r="R92" s="75"/>
+      <c r="S92" s="75"/>
+      <c r="T92" s="75"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+      <c r="X92"/>
+      <c r="Y92"/>
+      <c r="Z92"/>
+      <c r="AA92"/>
+      <c r="AB92"/>
+      <c r="AC92"/>
+      <c r="AD92"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N93" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="P93" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q93" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="P92" s="75" t="s">
+      <c r="R93" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="Q92" s="75" t="s">
-        <v>234</v>
-      </c>
-      <c r="R92" s="75" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="P93" s="75">
-        <f>SUMPRODUCT(R4:R81,Q4:Q81,$F4:$F81)</f>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P94" s="75">
+        <f>SUMPRODUCT(R4:R82,Q4:Q82,$F4:$F82)</f>
         <v>94.4</v>
       </c>
-      <c r="Q93" s="75">
-        <f t="shared" ref="Q93" si="9">SUMPRODUCT(S4:S81,R4:R81,$F4:$F81)</f>
-        <v>104.80000000000001</v>
-      </c>
-      <c r="R93" s="75">
-        <f>SUMPRODUCT(S4:S81,Q4:Q81,$F4:$F81)</f>
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="97" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA97" s="6"/>
-      <c r="AB97" s="6"/>
-      <c r="AC97" s="6"/>
-      <c r="AD97" s="6"/>
-    </row>
-    <row r="101" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA101" s="6"/>
-      <c r="AB101" s="6"/>
-      <c r="AC101" s="6"/>
-      <c r="AD101" s="6"/>
-    </row>
-    <row r="106" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA106" s="6"/>
-      <c r="AB106" s="6"/>
-      <c r="AC106" s="6"/>
-      <c r="AD106" s="6"/>
-    </row>
-    <row r="119" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA119" s="31"/>
-      <c r="AB119" s="31"/>
-      <c r="AC119" s="31"/>
-      <c r="AD119" s="31"/>
+      <c r="Q94" s="75">
+        <f t="shared" ref="Q94" si="7">SUMPRODUCT(S4:S82,R4:R82,$F4:$F82)</f>
+        <v>96.800000000000011</v>
+      </c>
+      <c r="R94" s="75">
+        <f>SUMPRODUCT(S4:S82,Q4:Q82,$F4:$F82)</f>
+        <v>85.199999999999989</v>
+      </c>
+    </row>
+    <row r="98" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA98" s="6"/>
+      <c r="AB98" s="6"/>
+      <c r="AC98" s="6"/>
+      <c r="AD98" s="6"/>
+    </row>
+    <row r="102" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA102" s="6"/>
+      <c r="AB102" s="6"/>
+      <c r="AC102" s="6"/>
+      <c r="AD102" s="6"/>
+    </row>
+    <row r="107" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA107" s="6"/>
+      <c r="AB107" s="6"/>
+      <c r="AC107" s="6"/>
+      <c r="AD107" s="6"/>
+    </row>
+    <row r="120" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA120" s="31"/>
+      <c r="AB120" s="31"/>
+      <c r="AC120" s="31"/>
+      <c r="AD120" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U81">
+  <conditionalFormatting sqref="B2:U82">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>